<commit_message>
finita la parte dei costi
</commit_message>
<xml_diff>
--- a/Documenti/Pianificazione/costo ruoli.xlsx
+++ b/Documenti/Pianificazione/costo ruoli.xlsx
@@ -1,38 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Foglio2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Foglio3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C30">
+    <comment ref="C38" authorId="0">
       <text>
         <r>
           <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="FF000000"/>
-            <sz val="11"/>
           </rPr>
-          <t xml:space="preserve">Più che “costo totale” non è questo il costo medio orario?</t>
+          <t>Più che “costo totale” non è questo il costo medio orario?</t>
         </r>
       </text>
     </comment>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>Ruolo</t>
   </si>
@@ -82,7 +81,7 @@
     <t>redazione Business Plan</t>
   </si>
   <si>
-    <t>PIANIFICAZIONE   </t>
+    <t>PIANIFICAZIONE</t>
   </si>
   <si>
     <t>studio software esistenti</t>
@@ -103,7 +102,7 @@
     <t>redazione della proposta</t>
   </si>
   <si>
-    <t>redazione manuale / consigli d'uso </t>
+    <t>redazione manuale / consigli d'uso</t>
   </si>
   <si>
     <t>presentazione proposta</t>
@@ -113,51 +112,45 @@
   </si>
   <si>
     <t>Costo totale</t>
+  </si>
+  <si>
+    <t>PROPSOTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-" numFmtId="165"/>
-    <numFmt formatCode="_-&quot;€ &quot;* #,##0.00_-;&quot;-€ &quot;* #,##0.00_-;_-&quot;€ &quot;* \-??_-;_-@_-" numFmtId="166"/>
-    <numFmt formatCode="&quot;€ &quot;#,##0.00;&quot;-€ &quot;#,##0.00" numFmtId="167"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;€ &quot;* #,##0.00_-;&quot;-€ &quot;* #,##0.00_-;_-&quot;€ &quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;€ &quot;#,##0.00;&quot;-€ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,198 +175,179 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="165">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-  </cellStyleXfs>
-  <cellXfs count="22">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="0" fontId="0" numFmtId="166" xfId="15">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="3" fontId="4" numFmtId="166" xfId="15">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="4" fontId="4" numFmtId="166" xfId="15">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -432,31 +406,319 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="25.42578125"/>
+    <col min="3" max="3" width="18.5703125"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,99 +726,91 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="3">
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="3">
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="3">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="3">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="3">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="3">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:I37"/>
+  <dimension ref="B2:I45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E41" activeCellId="0" pane="topLeft" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0040485829959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="44.85546875"/>
+    <col min="3" max="3" width="16.5703125"/>
+    <col min="4" max="4" width="21"/>
+    <col min="5" max="5" width="10.140625"/>
+    <col min="6" max="6" width="12.5703125"/>
+    <col min="7" max="7" width="14.85546875"/>
+    <col min="8" max="8" width="12"/>
+    <col min="9" max="9" width="11"/>
+    <col min="10" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.25" outlineLevel="0" r="2">
+    <row r="2" spans="2:9" ht="35.25" customHeight="1">
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -580,97 +834,97 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
+    <row r="3" spans="2:9">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="9">
         <v>5</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="9">
         <v>8</v>
       </c>
-      <c r="I3" s="10" t="n">
-        <f aca="false">E3*C32 +(H3*C35)</f>
+      <c r="I3" s="10">
+        <f>E3*C40 +(H3*C43)</f>
         <v>350</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="2:9">
       <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="9">
         <v>16</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="9">
         <v>6</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="10" t="n">
-        <f aca="false">E4*C32+F4*C34</f>
+      <c r="I4" s="10">
+        <f>E4*C40+F4*C42</f>
         <v>600</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="5">
+    <row r="5" spans="2:9">
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="9">
         <v>16</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="10" t="n">
-        <f aca="false">C5*C31+E5*C32</f>
+      <c r="I5" s="10">
+        <f>C5*C39+E5*C40</f>
         <v>520</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" spans="2:9">
       <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="12" t="n">
-        <f aca="false">SUM(C5)</f>
+      <c r="C6" s="12">
+        <f>SUM(C5)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <f aca="false">SUM(D3:D5)</f>
+      <c r="D6" s="3">
+        <f>SUM(D3:D5)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="n">
-        <f aca="false">SUM(E3:E5)</f>
+      <c r="E6" s="3">
+        <f>SUM(E3:E5)</f>
         <v>37</v>
       </c>
-      <c r="F6" s="3" t="n">
-        <f aca="false">SUM(F4:F5)</f>
+      <c r="F6" s="3">
+        <f>SUM(F4:F5)</f>
         <v>6</v>
       </c>
-      <c r="G6" s="3" t="n">
-        <f aca="false">SUM(G3:G5)</f>
+      <c r="G6" s="3">
+        <f>SUM(G3:G5)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="3" t="n">
-        <f aca="false">SUM(H3:H5)</f>
+      <c r="H6" s="3">
+        <f>SUM(H3:H5)</f>
         <v>8</v>
       </c>
-      <c r="I6" s="13" t="n">
-        <f aca="false">SUM(I3:I5)</f>
+      <c r="I6" s="13">
+        <f>SUM(I3:I5)</f>
         <v>1470</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" spans="2:9">
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -680,7 +934,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" spans="2:9">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -690,7 +944,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="10">
+    <row r="10" spans="2:9" ht="30">
       <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
         <v>2</v>
@@ -714,28 +968,28 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
+    <row r="11" spans="2:9">
       <c r="B11" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="9">
         <v>1</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="9">
         <v>24</v>
       </c>
-      <c r="H11" s="9" t="n">
+      <c r="H11" s="9">
         <v>23</v>
       </c>
-      <c r="I11" s="10" t="n">
-        <f aca="false">E11*C32+G11*C36+H11*C35</f>
+      <c r="I11" s="10">
+        <f>E11*C40+G11*C44+H11*C43</f>
         <v>965</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row r="12" spans="2:9">
       <c r="B12" s="18" t="s">
         <v>15</v>
       </c>
@@ -743,72 +997,72 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="9" t="n">
+      <c r="G12" s="9">
         <v>40</v>
       </c>
-      <c r="H12" s="9" t="n">
+      <c r="H12" s="9">
         <v>16</v>
       </c>
-      <c r="I12" s="10" t="n">
-        <f aca="false">G12*C36+H12*C35</f>
+      <c r="I12" s="10">
+        <f>G12*C44+H12*C43</f>
         <v>1000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row r="13" spans="2:9">
       <c r="B13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="9" t="n">
+      <c r="E13" s="9">
         <v>2</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="9" t="n">
+      <c r="G13" s="9">
         <v>5</v>
       </c>
-      <c r="H13" s="9" t="n">
+      <c r="H13" s="9">
         <v>8</v>
       </c>
-      <c r="I13" s="10" t="n">
-        <f aca="false">E13*C32+G13*C36+H13*C35</f>
+      <c r="I13" s="10">
+        <f>E13*C40+G13*C44+H13*C43</f>
         <v>335</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" spans="2:9">
       <c r="B14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="12" t="n">
-        <f aca="false">SUM(C6)</f>
+      <c r="C14" s="12">
+        <f>SUM(C6)</f>
         <v>1</v>
       </c>
-      <c r="D14" s="12" t="n">
-        <f aca="false">SUM(D6)</f>
+      <c r="D14" s="12">
+        <f>SUM(D6)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="12" t="n">
-        <f aca="false">SUM(E11:E13)</f>
+      <c r="E14" s="12">
+        <f>SUM(E11:E13)</f>
         <v>3</v>
       </c>
-      <c r="F14" s="12" t="n">
-        <f aca="false">SUM(F11:F13)</f>
+      <c r="F14" s="12">
+        <f>SUM(F11:F13)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="3" t="n">
-        <f aca="false">SUM(G11:G13)</f>
+      <c r="G14" s="3">
+        <f>SUM(G11:G13)</f>
         <v>69</v>
       </c>
-      <c r="H14" s="3" t="n">
-        <f aca="false">SUM(H11:H13)</f>
+      <c r="H14" s="3">
+        <f>SUM(H11:H13)</f>
         <v>47</v>
       </c>
-      <c r="I14" s="13" t="n">
-        <f aca="false">SUM(I11:I13)</f>
+      <c r="I14" s="13">
+        <f>SUM(I11:I13)</f>
         <v>2300</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" spans="2:9">
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -817,7 +1071,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" spans="2:9">
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -826,7 +1080,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
+    <row r="17" spans="2:9">
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -835,7 +1089,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30" outlineLevel="0" r="18">
+    <row r="18" spans="2:9" ht="30">
       <c r="B18" s="2"/>
       <c r="C18" s="4" t="s">
         <v>2</v>
@@ -859,49 +1113,49 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    <row r="19" spans="2:9">
       <c r="B19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="9" t="n">
+      <c r="E19" s="9">
         <v>3</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="9" t="n">
+      <c r="G19" s="9">
         <v>7</v>
       </c>
-      <c r="H19" s="9" t="n">
+      <c r="H19" s="9">
         <v>6</v>
       </c>
-      <c r="I19" s="10" t="n">
-        <f aca="false">E19*C32+G19*C36+H19*C35</f>
+      <c r="I19" s="10">
+        <f>E19*C40+G19*C44+H19*C43</f>
         <v>345</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+    <row r="20" spans="2:9">
       <c r="B20" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="8" t="n">
+      <c r="C20" s="8">
         <v>1</v>
       </c>
-      <c r="D20" s="9" t="n">
+      <c r="D20" s="9">
         <v>8</v>
       </c>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="9">
         <v>6</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="10" t="n">
-        <f aca="false">C20*C31+D20*C33+E20*C32</f>
+      <c r="I20" s="10">
+        <f>C20*C39+D20*C41+E20*C40</f>
         <v>420</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
+    <row r="21" spans="2:9">
       <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
@@ -909,174 +1163,259 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="9">
         <v>4</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="10" t="n">
-        <f aca="false">G21*C36</f>
+      <c r="I21" s="10">
+        <f>G21*C44</f>
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+    <row r="22" spans="2:9" ht="15.75" thickBot="1">
       <c r="B22" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="15"/>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="9">
         <v>2</v>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E22" s="9">
         <v>1</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
-      <c r="I22" s="10" t="n">
-        <f aca="false">D22*C33+E22*C32</f>
+      <c r="I22" s="10">
+        <f>D22*C41+E22*C40</f>
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
+    <row r="23" spans="2:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="B23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="12" t="n">
-        <f aca="false">SUM(C20:C22)</f>
+      <c r="C23" s="12">
+        <f>SUM(C20:C22)</f>
         <v>1</v>
       </c>
-      <c r="D23" s="3" t="n">
-        <f aca="false">SUM(D20:D22)</f>
+      <c r="D23" s="3">
+        <f>SUM(D20:D22)</f>
         <v>10</v>
       </c>
-      <c r="E23" s="3" t="n">
-        <f aca="false">SUM(E19:E22)</f>
+      <c r="E23" s="3">
+        <f>SUM(E19:E22)</f>
         <v>10</v>
       </c>
-      <c r="F23" s="3" t="n">
-        <f aca="false">SUM(F19:F23)</f>
+      <c r="F23" s="3">
+        <f ca="1">SUM(F19:F23)</f>
         <v>0</v>
       </c>
-      <c r="G23" s="3" t="n">
-        <f aca="false">SUM(G21:G22)</f>
+      <c r="G23" s="3">
+        <f>SUM(G21:G22)</f>
         <v>4</v>
       </c>
-      <c r="H23" s="3" t="n">
-        <f aca="false">SUM(H19:H22)</f>
+      <c r="H23" s="3">
+        <f>SUM(H19:H22)</f>
         <v>6</v>
       </c>
-      <c r="I23" s="13" t="n">
-        <f aca="false">SUM(I19:I22)</f>
+      <c r="I23" s="13">
+        <f>SUM(I19:I22)</f>
         <v>905</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
-      <c r="B27" s="20" t="s">
+    <row r="24" spans="2:9" ht="15.75" thickTop="1">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1</v>
+      </c>
+      <c r="D26" s="15">
+        <v>30</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="15">
+        <v>0</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="15">
+        <v>5</v>
+      </c>
+      <c r="D28" s="15">
+        <f>C28*30</f>
+        <v>150</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15">
+        <f>SUM(D26:D28)</f>
+        <v>180</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="21" t="n">
-        <f aca="false">I6+I14+I23</f>
-        <v>4675</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="B30" s="1" t="s">
+      <c r="C35" s="21">
+        <f>I6+I14+I23+D29</f>
+        <v>4855</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="B31" s="2" t="s">
+    <row r="39" spans="2:3">
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C39" s="3">
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="B32" s="2" t="s">
+    <row r="40" spans="2:3">
+      <c r="B40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C40" s="3">
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="B33" s="2" t="s">
+    <row r="41" spans="2:3">
+      <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C41" s="3">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="B34" s="2" t="s">
+    <row r="42" spans="2:3">
+      <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C42" s="3">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="B35" s="2" t="s">
+    <row r="43" spans="2:3">
+      <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C43" s="3">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="B36" s="2" t="s">
+    <row r="44" spans="2:3">
+      <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C44" s="3">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="B37" s="2" t="s">
+    <row r="45" spans="2:3">
+      <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C45" s="3">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>